<commit_message>
learning Day3 will be added to project
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyus\Desktop\Coding\RahulShetty_cypress\cypressAutomationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76A3BB6-3FC9-4B81-8701-5CAA762DB92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07DAFE2-8CAA-42A0-A701-7170285D9434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -226,6 +226,27 @@
   </si>
   <si>
     <t>cypress can handle hidden element by directly working with DOM, if we want to click an hidden element just force:true</t>
+  </si>
+  <si>
+    <t>.prop()</t>
+  </si>
+  <si>
+    <t>to get the properties of any element</t>
+  </si>
+  <si>
+    <t>By default cypress doesn't support frames, so we need to download iframe plugin</t>
+  </si>
+  <si>
+    <t>cy.frameLoaded(#frameID)</t>
+  </si>
+  <si>
+    <t>cy.iframe().find('Locator')</t>
+  </si>
+  <si>
+    <t>cy.get().filter(:contains("Nokia Edge"))</t>
+  </si>
+  <si>
+    <t>When handling calander always remember to get the desired values like date, month, year and click on the calander, look for the example</t>
   </si>
 </sst>
 </file>
@@ -555,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -847,6 +868,37 @@
         <v>66</v>
       </c>
     </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding excel data file
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyus\Desktop\Coding\RahulShetty_cypress\cypressAutomationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07DAFE2-8CAA-42A0-A701-7170285D9434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DC174B-FA16-4C28-BA1F-A0F95A700A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>